<commit_message>
Third quarter report plus some new codes
</commit_message>
<xml_diff>
--- a/Model/gene_comparison_09_30.xlsx
+++ b/Model/gene_comparison_09_30.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="60" windowWidth="21060" windowHeight="10848"/>
+    <workbookView xWindow="384" yWindow="60" windowWidth="15576" windowHeight="9816"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="611">
   <si>
     <t>mmp0003</t>
   </si>
@@ -1841,6 +1841,12 @@
   </si>
   <si>
     <t>Proposal for Our Model</t>
+  </si>
+  <si>
+    <t>KEGG</t>
+  </si>
+  <si>
+    <t>http://www.genome.jp/dbget-bin/www_bget?mmp:MMP0002</t>
   </si>
 </sst>
 </file>
@@ -2182,10 +2188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D391"/>
+  <dimension ref="A1:E391"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2194,10 +2200,11 @@
     <col min="2" max="2" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="53" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>605</v>
       </c>
@@ -2210,8 +2217,11 @@
       <c r="D1" s="1" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2221,8 +2231,11 @@
       <c r="C2" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2233,7 +2246,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2244,7 +2257,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2255,7 +2268,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2266,7 +2279,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2277,7 +2290,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2288,7 +2301,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2299,7 +2312,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2310,7 +2323,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2321,7 +2334,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2332,7 +2345,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2343,7 +2356,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2354,7 +2367,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2365,7 +2378,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>